<commit_message>
Avance Req1 Ordenamientos Recursivos - Reto 1
</commit_message>
<xml_diff>
--- a/Docs/VC -Tablas de Datos.xlsx
+++ b/Docs/VC -Tablas de Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentina/Desktop/EDA - Lab/Reto1-G04/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2461D530-6627-FA40-BCB3-6DC062D155D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1334CBB-A32F-FF45-98B3-D88D604700B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="1120" yWindow="2040" windowWidth="25780" windowHeight="15580" firstSheet="4" activeTab="6" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4-5" sheetId="1" r:id="rId1"/>
@@ -10590,7 +10590,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0"/>
+    <sheetView zoomScale="115" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10601,7 +10601,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0"/>
+    <sheetView zoomScale="96" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10612,7 +10612,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10623,7 +10623,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10634,7 +10634,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10645,7 +10645,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C0D6BB1E-4928-4857-A0CD-C818D0A5A6F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10656,7 +10656,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B3AE6AD4-6EB7-44ED-A987-5D4A68E7E10B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11224,7 +11224,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E15" sqref="E15:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>